<commit_message>
[FIX]: Messed up spreadsheet is now fixed
</commit_message>
<xml_diff>
--- a/210427_123816.xlsx
+++ b/210427_123816.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Documents\Programs\python\french\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E915A9-98F7-4EA3-BE03-B27747FED765}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3587002E-AA67-49AA-AD0D-A3D0C633685E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="408" yWindow="181" windowWidth="14037" windowHeight="11158" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11622" yWindow="692" windowWidth="14037" windowHeight="11157" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Automated" sheetId="2" r:id="rId1"/>
@@ -18899,8 +18899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB1732"/>
   <sheetViews>
-    <sheetView topLeftCell="A666" workbookViewId="0">
-      <selection activeCell="C686" sqref="C686"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.2" x14ac:dyDescent="0.3"/>
@@ -40816,7 +40816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B488"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A418" workbookViewId="0"/>
+    <sheetView topLeftCell="A131" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.2" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>